<commit_message>
Commit - 27-12-2018 - 002
</commit_message>
<xml_diff>
--- a/R4-1/templates/Provar Regression RWH/Provar Regression RWH_Test1_Transfer1.xlsx
+++ b/R4-1/templates/Provar Regression RWH/Provar Regression RWH_Test1_Transfer1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Incapsulate\Provar\R4-1\R4-1\templates\Provar Regression RWH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Incapsulate\git\Jenkins-Provar-test\R4-1\templates\Provar Regression RWH\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{29FE1033-6104-4C5B-B28A-6DDCA5BA20BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -36,9 +37,6 @@
     <t>questionLabel</t>
   </si>
   <si>
-    <t>Animal size</t>
-  </si>
-  <si>
     <t>singlePicklistMatrix</t>
   </si>
   <si>
@@ -163,12 +161,15 @@
   </si>
   <si>
     <t>(555) 555-5555</t>
+  </si>
+  <si>
+    <t>Animal Size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -564,23 +565,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" activeCellId="1" sqref="A9:XFD9 A11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.21875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="26.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" style="5"/>
-    <col min="4" max="4" width="26.21875" style="6"/>
-    <col min="5" max="16384" width="26.21875" style="3"/>
+    <col min="1" max="1" width="29.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" style="5"/>
+    <col min="4" max="4" width="26.1796875" style="6"/>
+    <col min="5" max="16384" width="26.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.8">
+    <row r="1" spans="1:4" ht="14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,182 +595,182 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13.8">
+    <row r="2" spans="1:4" ht="14">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2"/>
       <c r="B3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="26.4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="25">
       <c r="A4" s="2"/>
       <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="26.4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="25">
       <c r="A6" s="2"/>
       <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2"/>
       <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="25">
+      <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="26.4">
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="92.4">
+    </row>
+    <row r="10" spans="1:4" ht="87.5">
       <c r="A10" s="2"/>
       <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2"/>
       <c r="B11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2"/>
       <c r="B12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="39.6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="37.5">
       <c r="A13" s="2"/>
       <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="25">
+      <c r="B14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26.4">
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="D14" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>